<commit_message>
Tidied up turn delay trendline excel file. Also added comment headers for the functions in main.ino.
</commit_message>
<xml_diff>
--- a/trendline_for_turn_delay.xlsx
+++ b/trendline_for_turn_delay.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15990" windowHeight="8370"/>
+    <workbookView windowWidth="15990" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2">
   <si>
     <t>dist</t>
   </si>
   <si>
     <t>time</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -30,16 +27,39 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -59,6 +79,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -67,39 +94,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -114,61 +118,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,6 +138,53 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -198,187 +195,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,17 +389,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -425,6 +418,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -440,13 +448,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -474,27 +486,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -512,130 +509,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -810,10 +807,10 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-0.282258064516129"/>
-                  <c:y val="0.0173611111111111"/>
+                  <c:y val="0.0104166666666667"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="#,##0.0000000_);[Red]\(#,##0.0000000\)" sourceLinked="0"/>
+              <c:numFmt formatCode="0.0000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -1931,13 +1928,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="10.5714285714286"/>
     <col min="2" max="2" width="14"/>
@@ -1945,32 +1942,20 @@
     <col min="11" max="11" width="11.7142857142857"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>150</v>
       </c>
       <c r="B2" s="1">
         <v>1500</v>
-      </c>
-      <c r="I2">
-        <v>4218075</v>
-      </c>
-      <c r="J2">
-        <v>300</v>
-      </c>
-      <c r="K2">
-        <v>-1.585</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1981,12 +1966,6 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="9:9">
-      <c r="I4">
-        <f>I2*(J2^K2)</f>
-        <v>499.893061462152</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>